<commit_message>
updates in elisa sheet
</commit_message>
<xml_diff>
--- a/DATA/elisa_data_serial_dilution.xlsx
+++ b/DATA/elisa_data_serial_dilution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarudutt/Documents/impac-tb-r/CODING-TEAM-BOOKDOWN-/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA859239-A860-B445-9B02-50115A77E3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD27415-B9DA-AB49-BD8A-242364B5F3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16480" xr2:uid="{AA96C3F1-C4D8-0F49-9B50-9F673D3A8DC2}"/>
   </bookViews>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF21CEE-201D-2545-A0DA-F5B78BD5039D}">
   <dimension ref="B6:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="176" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="176" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,7 +685,7 @@
         <v>0.26</v>
       </c>
       <c r="H15">
-        <v>28</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
@@ -915,7 +915,7 @@
         <v>0.16</v>
       </c>
       <c r="H25">
-        <v>18</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">

</xml_diff>